<commit_message>
Added time for 15-02-2016 group work
</commit_message>
<xml_diff>
--- a/Uurbesteding.xlsx
+++ b/Uurbesteding.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="24">
   <si>
     <t>studie</t>
   </si>
@@ -50,6 +50,42 @@
   </si>
   <si>
     <t>totaal</t>
+  </si>
+  <si>
+    <t>week 4</t>
+  </si>
+  <si>
+    <t>week 5</t>
+  </si>
+  <si>
+    <t>week 6</t>
+  </si>
+  <si>
+    <t>week 7</t>
+  </si>
+  <si>
+    <t>week 8</t>
+  </si>
+  <si>
+    <t>week 9</t>
+  </si>
+  <si>
+    <t>week 10</t>
+  </si>
+  <si>
+    <t>week 11</t>
+  </si>
+  <si>
+    <t>week 12</t>
+  </si>
+  <si>
+    <t>week 13</t>
+  </si>
+  <si>
+    <t>week 14</t>
+  </si>
+  <si>
+    <t>week 15</t>
   </si>
 </sst>
 </file>
@@ -57,7 +93,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="h:mm;@"/>
+    <numFmt numFmtId="164" formatCode="h:mm;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -210,7 +246,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Accent2" xfId="1" builtinId="33"/>
@@ -519,10 +555,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:Q15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -531,7 +567,7 @@
     <col min="2" max="2" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="12"/>
       <c r="B1" s="13"/>
       <c r="C1" s="11" t="s">
@@ -543,8 +579,44 @@
       <c r="E1" s="11" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="L1" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="M1" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="N1" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="O1" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="P1" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q1" s="11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -556,8 +628,20 @@
       </c>
       <c r="D2" s="18"/>
       <c r="E2" s="18"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="18"/>
+      <c r="L2" s="18"/>
+      <c r="M2" s="18"/>
+      <c r="N2" s="18"/>
+      <c r="O2" s="18"/>
+      <c r="P2" s="18"/>
+      <c r="Q2" s="18"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="9" t="s">
         <v>2</v>
@@ -567,8 +651,20 @@
       </c>
       <c r="D3" s="18"/>
       <c r="E3" s="18"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="18"/>
+      <c r="L3" s="18"/>
+      <c r="M3" s="18"/>
+      <c r="N3" s="18"/>
+      <c r="O3" s="18"/>
+      <c r="P3" s="18"/>
+      <c r="Q3" s="18"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="9" t="s">
         <v>3</v>
@@ -578,8 +674,20 @@
       </c>
       <c r="D4" s="18"/>
       <c r="E4" s="18"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="18"/>
+      <c r="I4" s="18"/>
+      <c r="J4" s="18"/>
+      <c r="K4" s="18"/>
+      <c r="L4" s="18"/>
+      <c r="M4" s="18"/>
+      <c r="N4" s="18"/>
+      <c r="O4" s="18"/>
+      <c r="P4" s="18"/>
+      <c r="Q4" s="18"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="9" t="s">
         <v>4</v>
@@ -589,8 +697,20 @@
       </c>
       <c r="D5" s="18"/>
       <c r="E5" s="18"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5" s="18"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="18"/>
+      <c r="I5" s="18"/>
+      <c r="J5" s="18"/>
+      <c r="K5" s="18"/>
+      <c r="L5" s="18"/>
+      <c r="M5" s="18"/>
+      <c r="N5" s="18"/>
+      <c r="O5" s="18"/>
+      <c r="P5" s="18"/>
+      <c r="Q5" s="18"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
@@ -602,8 +722,20 @@
       </c>
       <c r="D6" s="18"/>
       <c r="E6" s="18"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="18"/>
+      <c r="K6" s="18"/>
+      <c r="L6" s="18"/>
+      <c r="M6" s="18"/>
+      <c r="N6" s="18"/>
+      <c r="O6" s="18"/>
+      <c r="P6" s="18"/>
+      <c r="Q6" s="18"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
       <c r="B7" s="10" t="s">
         <v>2</v>
@@ -613,8 +745,20 @@
       </c>
       <c r="D7" s="18"/>
       <c r="E7" s="18"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7" s="18"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="18"/>
+      <c r="J7" s="18"/>
+      <c r="K7" s="18"/>
+      <c r="L7" s="18"/>
+      <c r="M7" s="18"/>
+      <c r="N7" s="18"/>
+      <c r="O7" s="18"/>
+      <c r="P7" s="18"/>
+      <c r="Q7" s="18"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
       <c r="B8" s="10" t="s">
         <v>3</v>
@@ -624,8 +768,20 @@
       </c>
       <c r="D8" s="18"/>
       <c r="E8" s="18"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="18"/>
+      <c r="I8" s="18"/>
+      <c r="J8" s="18"/>
+      <c r="K8" s="18"/>
+      <c r="L8" s="18"/>
+      <c r="M8" s="18"/>
+      <c r="N8" s="18"/>
+      <c r="O8" s="18"/>
+      <c r="P8" s="18"/>
+      <c r="Q8" s="18"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
       <c r="B9" s="10" t="s">
         <v>6</v>
@@ -635,8 +791,20 @@
       </c>
       <c r="D9" s="18"/>
       <c r="E9" s="18"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="18"/>
+      <c r="J9" s="18"/>
+      <c r="K9" s="18"/>
+      <c r="L9" s="18"/>
+      <c r="M9" s="18"/>
+      <c r="N9" s="18"/>
+      <c r="O9" s="18"/>
+      <c r="P9" s="18"/>
+      <c r="Q9" s="18"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>8</v>
       </c>
@@ -644,15 +812,29 @@
       <c r="C10" s="18">
         <v>0</v>
       </c>
-      <c r="D10" s="18"/>
+      <c r="D10" s="18">
+        <v>0.17708333333333334</v>
+      </c>
       <c r="E10" s="18"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="18"/>
+      <c r="J10" s="18"/>
+      <c r="K10" s="18"/>
+      <c r="L10" s="18"/>
+      <c r="M10" s="18"/>
+      <c r="N10" s="18"/>
+      <c r="O10" s="18"/>
+      <c r="P10" s="18"/>
+      <c r="Q10" s="18"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C11" s="18"/>
       <c r="D11" s="18"/>
       <c r="E11" s="18"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
         <v>11</v>
       </c>
@@ -665,14 +847,62 @@
       </c>
       <c r="D12" s="18">
         <f t="shared" ref="D12:E12" si="0">D10+D6+D2</f>
-        <v>0</v>
+        <v>0.17708333333333334</v>
       </c>
       <c r="E12" s="18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F12" s="18">
+        <f t="shared" ref="F12:Q12" si="1">F10+F6+F2</f>
+        <v>0</v>
+      </c>
+      <c r="G12" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H12" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I12" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J12" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K12" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L12" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M12" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N12" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O12" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P12" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q12" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="15"/>
       <c r="B13" s="17" t="s">
         <v>2</v>
@@ -682,15 +912,63 @@
         <v>0.25</v>
       </c>
       <c r="D13" s="18">
-        <f t="shared" ref="D13:E13" si="1">D10+D7+D3</f>
-        <v>0</v>
+        <f t="shared" ref="D13:E13" si="2">D10+D7+D3</f>
+        <v>0.17708333333333334</v>
       </c>
       <c r="E13" s="18">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F13" s="18">
+        <f t="shared" ref="F13:Q13" si="3">F10+F7+F3</f>
+        <v>0</v>
+      </c>
+      <c r="G13" s="18">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="H13" s="18">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I13" s="18">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J13" s="18">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K13" s="18">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L13" s="18">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M13" s="18">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="N13" s="18">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="O13" s="18">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="P13" s="18">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="Q13" s="18">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="15"/>
       <c r="B14" s="17" t="s">
         <v>3</v>
@@ -700,15 +978,63 @@
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="D14" s="18">
-        <f t="shared" ref="D14:E14" si="2">D10+D8+D4</f>
-        <v>0</v>
+        <f t="shared" ref="D14:E14" si="4">D10+D8+D4</f>
+        <v>0.17708333333333334</v>
       </c>
       <c r="E14" s="18">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F14" s="18">
+        <f t="shared" ref="F14:Q14" si="5">F10+F8+F4</f>
+        <v>0</v>
+      </c>
+      <c r="G14" s="18">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="H14" s="18">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="I14" s="18">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J14" s="18">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K14" s="18">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L14" s="18">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="M14" s="18">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="N14" s="18">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O14" s="18">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="P14" s="18">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="Q14" s="18">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="16"/>
       <c r="B15" s="17" t="s">
         <v>6</v>
@@ -718,11 +1044,59 @@
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="D15" s="18">
-        <f t="shared" ref="D15:E15" si="3">D10+D9+D5</f>
-        <v>0</v>
+        <f t="shared" ref="D15:E15" si="6">D10+D9+D5</f>
+        <v>0.17708333333333334</v>
       </c>
       <c r="E15" s="18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="F15" s="18">
+        <f t="shared" ref="F15:Q15" si="7">F10+F9+F5</f>
+        <v>0</v>
+      </c>
+      <c r="G15" s="18">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="H15" s="18">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="I15" s="18">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="J15" s="18">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="K15" s="18">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="L15" s="18">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="M15" s="18">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="N15" s="18">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="O15" s="18">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="P15" s="18">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="Q15" s="18">
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
reformatted numbers to the correct [h]:mm format for time calculations
</commit_message>
<xml_diff>
--- a/Uurbesteding.xlsx
+++ b/Uurbesteding.xlsx
@@ -93,9 +93,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="h:mm;@"/>
+    <numFmt numFmtId="169" formatCode="[h]:mm"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -109,6 +109,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF222426"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="6">
@@ -227,7 +233,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="2" applyBorder="1"/>
@@ -246,7 +252,8 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Accent2" xfId="1" builtinId="33"/>
@@ -555,10 +562,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q15"/>
+  <dimension ref="A1:Q19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -623,92 +630,92 @@
       <c r="B2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="18">
+      <c r="C2" s="19">
         <v>0.25</v>
       </c>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
-      <c r="J2" s="18"/>
-      <c r="K2" s="18"/>
-      <c r="L2" s="18"/>
-      <c r="M2" s="18"/>
-      <c r="N2" s="18"/>
-      <c r="O2" s="18"/>
-      <c r="P2" s="18"/>
-      <c r="Q2" s="18"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
+      <c r="K2" s="19"/>
+      <c r="L2" s="19"/>
+      <c r="M2" s="19"/>
+      <c r="N2" s="19"/>
+      <c r="O2" s="19"/>
+      <c r="P2" s="19"/>
+      <c r="Q2" s="19"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="18">
+      <c r="C3" s="19">
         <v>0.25</v>
       </c>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18"/>
-      <c r="I3" s="18"/>
-      <c r="J3" s="18"/>
-      <c r="K3" s="18"/>
-      <c r="L3" s="18"/>
-      <c r="M3" s="18"/>
-      <c r="N3" s="18"/>
-      <c r="O3" s="18"/>
-      <c r="P3" s="18"/>
-      <c r="Q3" s="18"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
+      <c r="K3" s="19"/>
+      <c r="L3" s="19"/>
+      <c r="M3" s="19"/>
+      <c r="N3" s="19"/>
+      <c r="O3" s="19"/>
+      <c r="P3" s="19"/>
+      <c r="Q3" s="19"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="18">
+      <c r="C4" s="19">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="18"/>
-      <c r="J4" s="18"/>
-      <c r="K4" s="18"/>
-      <c r="L4" s="18"/>
-      <c r="M4" s="18"/>
-      <c r="N4" s="18"/>
-      <c r="O4" s="18"/>
-      <c r="P4" s="18"/>
-      <c r="Q4" s="18"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="19"/>
+      <c r="J4" s="19"/>
+      <c r="K4" s="19"/>
+      <c r="L4" s="19"/>
+      <c r="M4" s="19"/>
+      <c r="N4" s="19"/>
+      <c r="O4" s="19"/>
+      <c r="P4" s="19"/>
+      <c r="Q4" s="19"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="18">
+      <c r="C5" s="19">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="18"/>
-      <c r="I5" s="18"/>
-      <c r="J5" s="18"/>
-      <c r="K5" s="18"/>
-      <c r="L5" s="18"/>
-      <c r="M5" s="18"/>
-      <c r="N5" s="18"/>
-      <c r="O5" s="18"/>
-      <c r="P5" s="18"/>
-      <c r="Q5" s="18"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="19"/>
+      <c r="J5" s="19"/>
+      <c r="K5" s="19"/>
+      <c r="L5" s="19"/>
+      <c r="M5" s="19"/>
+      <c r="N5" s="19"/>
+      <c r="O5" s="19"/>
+      <c r="P5" s="19"/>
+      <c r="Q5" s="19"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
@@ -717,122 +724,134 @@
       <c r="B6" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="18">
-        <v>0</v>
-      </c>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="18"/>
-      <c r="J6" s="18"/>
-      <c r="K6" s="18"/>
-      <c r="L6" s="18"/>
-      <c r="M6" s="18"/>
-      <c r="N6" s="18"/>
-      <c r="O6" s="18"/>
-      <c r="P6" s="18"/>
-      <c r="Q6" s="18"/>
+      <c r="C6" s="19">
+        <v>0</v>
+      </c>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="19"/>
+      <c r="K6" s="19"/>
+      <c r="L6" s="19"/>
+      <c r="M6" s="19"/>
+      <c r="N6" s="19"/>
+      <c r="O6" s="19"/>
+      <c r="P6" s="19"/>
+      <c r="Q6" s="19"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
       <c r="B7" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="18">
-        <v>0</v>
-      </c>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18"/>
-      <c r="I7" s="18"/>
-      <c r="J7" s="18"/>
-      <c r="K7" s="18"/>
-      <c r="L7" s="18"/>
-      <c r="M7" s="18"/>
-      <c r="N7" s="18"/>
-      <c r="O7" s="18"/>
-      <c r="P7" s="18"/>
-      <c r="Q7" s="18"/>
+      <c r="C7" s="19">
+        <v>0</v>
+      </c>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="19"/>
+      <c r="J7" s="19"/>
+      <c r="K7" s="19"/>
+      <c r="L7" s="19"/>
+      <c r="M7" s="19"/>
+      <c r="N7" s="19"/>
+      <c r="O7" s="19"/>
+      <c r="P7" s="19"/>
+      <c r="Q7" s="19"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
       <c r="B8" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="18">
-        <v>0</v>
-      </c>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="18"/>
-      <c r="I8" s="18"/>
-      <c r="J8" s="18"/>
-      <c r="K8" s="18"/>
-      <c r="L8" s="18"/>
-      <c r="M8" s="18"/>
-      <c r="N8" s="18"/>
-      <c r="O8" s="18"/>
-      <c r="P8" s="18"/>
-      <c r="Q8" s="18"/>
+      <c r="C8" s="19">
+        <v>0</v>
+      </c>
+      <c r="D8" s="19"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="19"/>
+      <c r="I8" s="19"/>
+      <c r="J8" s="19"/>
+      <c r="K8" s="19"/>
+      <c r="L8" s="19"/>
+      <c r="M8" s="19"/>
+      <c r="N8" s="19"/>
+      <c r="O8" s="19"/>
+      <c r="P8" s="19"/>
+      <c r="Q8" s="19"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
       <c r="B9" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="18">
-        <v>0</v>
-      </c>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="18"/>
-      <c r="I9" s="18"/>
-      <c r="J9" s="18"/>
-      <c r="K9" s="18"/>
-      <c r="L9" s="18"/>
-      <c r="M9" s="18"/>
-      <c r="N9" s="18"/>
-      <c r="O9" s="18"/>
-      <c r="P9" s="18"/>
-      <c r="Q9" s="18"/>
+      <c r="C9" s="19">
+        <v>0</v>
+      </c>
+      <c r="D9" s="19"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="19"/>
+      <c r="J9" s="19"/>
+      <c r="K9" s="19"/>
+      <c r="L9" s="19"/>
+      <c r="M9" s="19"/>
+      <c r="N9" s="19"/>
+      <c r="O9" s="19"/>
+      <c r="P9" s="19"/>
+      <c r="Q9" s="19"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="8"/>
-      <c r="C10" s="18">
-        <v>0</v>
-      </c>
-      <c r="D10" s="18">
+      <c r="C10" s="19">
+        <v>0</v>
+      </c>
+      <c r="D10" s="19">
         <v>0.17708333333333334</v>
       </c>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="18"/>
-      <c r="I10" s="18"/>
-      <c r="J10" s="18"/>
-      <c r="K10" s="18"/>
-      <c r="L10" s="18"/>
-      <c r="M10" s="18"/>
-      <c r="N10" s="18"/>
-      <c r="O10" s="18"/>
-      <c r="P10" s="18"/>
-      <c r="Q10" s="18"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="19"/>
+      <c r="J10" s="19"/>
+      <c r="K10" s="19"/>
+      <c r="L10" s="19"/>
+      <c r="M10" s="19"/>
+      <c r="N10" s="19"/>
+      <c r="O10" s="19"/>
+      <c r="P10" s="19"/>
+      <c r="Q10" s="19"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="C11" s="18"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="19"/>
+      <c r="I11" s="19"/>
+      <c r="J11" s="19"/>
+      <c r="K11" s="19"/>
+      <c r="L11" s="19"/>
+      <c r="M11" s="19"/>
+      <c r="N11" s="19"/>
+      <c r="O11" s="19"/>
+      <c r="P11" s="19"/>
+      <c r="Q11" s="19"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
@@ -841,63 +860,63 @@
       <c r="B12" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="18">
+      <c r="C12" s="19">
         <f>C10+C6+C2</f>
         <v>0.25</v>
       </c>
-      <c r="D12" s="18">
+      <c r="D12" s="19">
         <f t="shared" ref="D12:E12" si="0">D10+D6+D2</f>
         <v>0.17708333333333334</v>
       </c>
-      <c r="E12" s="18">
+      <c r="E12" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F12" s="18">
+      <c r="F12" s="19">
         <f t="shared" ref="F12:Q12" si="1">F10+F6+F2</f>
         <v>0</v>
       </c>
-      <c r="G12" s="18">
+      <c r="G12" s="19">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H12" s="18">
+      <c r="H12" s="19">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I12" s="18">
+      <c r="I12" s="19">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J12" s="18">
+      <c r="J12" s="19">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K12" s="18">
+      <c r="K12" s="19">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L12" s="18">
+      <c r="L12" s="19">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M12" s="18">
+      <c r="M12" s="19">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="N12" s="18">
+      <c r="N12" s="19">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O12" s="18">
+      <c r="O12" s="19">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="P12" s="18">
+      <c r="P12" s="19">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Q12" s="18">
+      <c r="Q12" s="19">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -907,63 +926,63 @@
       <c r="B13" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="C13" s="18">
+      <c r="C13" s="19">
         <f>C10+C7+C3</f>
         <v>0.25</v>
       </c>
-      <c r="D13" s="18">
+      <c r="D13" s="19">
         <f t="shared" ref="D13:E13" si="2">D10+D7+D3</f>
         <v>0.17708333333333334</v>
       </c>
-      <c r="E13" s="18">
+      <c r="E13" s="19">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F13" s="18">
+      <c r="F13" s="19">
         <f t="shared" ref="F13:Q13" si="3">F10+F7+F3</f>
         <v>0</v>
       </c>
-      <c r="G13" s="18">
+      <c r="G13" s="19">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="H13" s="18">
+      <c r="H13" s="19">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="I13" s="18">
+      <c r="I13" s="19">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J13" s="18">
+      <c r="J13" s="19">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="K13" s="18">
+      <c r="K13" s="19">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="L13" s="18">
+      <c r="L13" s="19">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M13" s="18">
+      <c r="M13" s="19">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="N13" s="18">
+      <c r="N13" s="19">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="O13" s="18">
+      <c r="O13" s="19">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="P13" s="18">
+      <c r="P13" s="19">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="Q13" s="18">
+      <c r="Q13" s="19">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -973,63 +992,63 @@
       <c r="B14" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="C14" s="18">
+      <c r="C14" s="19">
         <f>C10+C8+C4</f>
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="D14" s="18">
+      <c r="D14" s="19">
         <f t="shared" ref="D14:E14" si="4">D10+D8+D4</f>
         <v>0.17708333333333334</v>
       </c>
-      <c r="E14" s="18">
+      <c r="E14" s="19">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="F14" s="18">
+      <c r="F14" s="19">
         <f t="shared" ref="F14:Q14" si="5">F10+F8+F4</f>
         <v>0</v>
       </c>
-      <c r="G14" s="18">
+      <c r="G14" s="19">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="H14" s="18">
+      <c r="H14" s="19">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="I14" s="18">
+      <c r="I14" s="19">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="J14" s="18">
+      <c r="J14" s="19">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="K14" s="18">
+      <c r="K14" s="19">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="L14" s="18">
+      <c r="L14" s="19">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="M14" s="18">
+      <c r="M14" s="19">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="N14" s="18">
+      <c r="N14" s="19">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="O14" s="18">
+      <c r="O14" s="19">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="P14" s="18">
+      <c r="P14" s="19">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="Q14" s="18">
+      <c r="Q14" s="19">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -1039,66 +1058,72 @@
       <c r="B15" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="18">
+      <c r="C15" s="19">
         <f>C10+C9+C5</f>
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="D15" s="18">
+      <c r="D15" s="19">
         <f t="shared" ref="D15:E15" si="6">D10+D9+D5</f>
         <v>0.17708333333333334</v>
       </c>
-      <c r="E15" s="18">
+      <c r="E15" s="19">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="F15" s="18">
+      <c r="F15" s="19">
         <f t="shared" ref="F15:Q15" si="7">F10+F9+F5</f>
         <v>0</v>
       </c>
-      <c r="G15" s="18">
+      <c r="G15" s="19">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="H15" s="18">
+      <c r="H15" s="19">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="I15" s="18">
+      <c r="I15" s="19">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="J15" s="18">
+      <c r="J15" s="19">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="K15" s="18">
+      <c r="K15" s="19">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="L15" s="18">
+      <c r="L15" s="19">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="M15" s="18">
+      <c r="M15" s="19">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="N15" s="18">
+      <c r="N15" s="19">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="O15" s="18">
+      <c r="O15" s="19">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="P15" s="18">
+      <c r="P15" s="19">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="Q15" s="18">
+      <c r="Q15" s="19">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="18"/>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added uren voor groepswer 17-02-2016
</commit_message>
<xml_diff>
--- a/Uurbesteding.xlsx
+++ b/Uurbesteding.xlsx
@@ -93,7 +93,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="[h]:mm"/>
+    <numFmt numFmtId="164" formatCode="[h]:mm"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -252,8 +252,8 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Accent2" xfId="1" builtinId="33"/>
@@ -565,7 +565,7 @@
   <dimension ref="A1:Q19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -820,7 +820,7 @@
         <v>0</v>
       </c>
       <c r="D10" s="19">
-        <v>0.17708333333333334</v>
+        <v>0.34375</v>
       </c>
       <c r="E10" s="19"/>
       <c r="F10" s="19"/>
@@ -866,7 +866,7 @@
       </c>
       <c r="D12" s="19">
         <f t="shared" ref="D12:E12" si="0">D10+D6+D2</f>
-        <v>0.17708333333333334</v>
+        <v>0.34375</v>
       </c>
       <c r="E12" s="19">
         <f t="shared" si="0"/>
@@ -932,7 +932,7 @@
       </c>
       <c r="D13" s="19">
         <f t="shared" ref="D13:E13" si="2">D10+D7+D3</f>
-        <v>0.17708333333333334</v>
+        <v>0.34375</v>
       </c>
       <c r="E13" s="19">
         <f t="shared" si="2"/>
@@ -998,7 +998,7 @@
       </c>
       <c r="D14" s="19">
         <f t="shared" ref="D14:E14" si="4">D10+D8+D4</f>
-        <v>0.17708333333333334</v>
+        <v>0.34375</v>
       </c>
       <c r="E14" s="19">
         <f t="shared" si="4"/>
@@ -1064,7 +1064,7 @@
       </c>
       <c r="D15" s="19">
         <f t="shared" ref="D15:E15" si="6">D10+D9+D5</f>
-        <v>0.17708333333333334</v>
+        <v>0.34375</v>
       </c>
       <c r="E15" s="19">
         <f t="shared" si="6"/>

</xml_diff>

<commit_message>
Added 1 hour to group time of 17-02-2016
</commit_message>
<xml_diff>
--- a/Uurbesteding.xlsx
+++ b/Uurbesteding.xlsx
@@ -565,7 +565,7 @@
   <dimension ref="A1:Q19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -820,7 +820,7 @@
         <v>0</v>
       </c>
       <c r="D10" s="19">
-        <v>0.34375</v>
+        <v>0.38541666666666669</v>
       </c>
       <c r="E10" s="19"/>
       <c r="F10" s="19"/>
@@ -866,7 +866,7 @@
       </c>
       <c r="D12" s="19">
         <f t="shared" ref="D12:E12" si="0">D10+D6+D2</f>
-        <v>0.34375</v>
+        <v>0.38541666666666669</v>
       </c>
       <c r="E12" s="19">
         <f t="shared" si="0"/>
@@ -932,7 +932,7 @@
       </c>
       <c r="D13" s="19">
         <f t="shared" ref="D13:E13" si="2">D10+D7+D3</f>
-        <v>0.34375</v>
+        <v>0.38541666666666669</v>
       </c>
       <c r="E13" s="19">
         <f t="shared" si="2"/>
@@ -998,7 +998,7 @@
       </c>
       <c r="D14" s="19">
         <f t="shared" ref="D14:E14" si="4">D10+D8+D4</f>
-        <v>0.34375</v>
+        <v>0.38541666666666669</v>
       </c>
       <c r="E14" s="19">
         <f t="shared" si="4"/>
@@ -1064,7 +1064,7 @@
       </c>
       <c r="D15" s="19">
         <f t="shared" ref="D15:E15" si="6">D10+D9+D5</f>
-        <v>0.34375</v>
+        <v>0.38541666666666669</v>
       </c>
       <c r="E15" s="19">
         <f t="shared" si="6"/>

</xml_diff>

<commit_message>
Added some time to private coding
</commit_message>
<xml_diff>
--- a/Uurbesteding.xlsx
+++ b/Uurbesteding.xlsx
@@ -565,7 +565,7 @@
   <dimension ref="A1:Q19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -727,7 +727,9 @@
       <c r="C6" s="19">
         <v>0</v>
       </c>
-      <c r="D6" s="19"/>
+      <c r="D6" s="19">
+        <v>0.125</v>
+      </c>
       <c r="E6" s="19"/>
       <c r="F6" s="19"/>
       <c r="G6" s="19"/>
@@ -866,7 +868,7 @@
       </c>
       <c r="D12" s="19">
         <f t="shared" ref="D12:E12" si="0">D10+D6+D2</f>
-        <v>0.38541666666666669</v>
+        <v>0.51041666666666674</v>
       </c>
       <c r="E12" s="19">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
Added own hours of work time
</commit_message>
<xml_diff>
--- a/Uurbesteding.xlsx
+++ b/Uurbesteding.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="26812"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Mathias/Desktop/SwOp-Group03/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="20420" windowHeight="11940"/>
+    <workbookView xWindow="240" yWindow="465" windowWidth="20415" windowHeight="11940"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -270,7 +265,7 @@
     <cellStyle name="Accent3" xfId="2" builtinId="37"/>
     <cellStyle name="Accent4" xfId="3" builtinId="41"/>
     <cellStyle name="Accent6" xfId="4" builtinId="49"/>
-    <cellStyle name="Stand." xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -575,16 +570,16 @@
   <dimension ref="A1:Q19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5" customWidth="1"/>
+    <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="12"/>
       <c r="B1" s="13"/>
       <c r="C1" s="11" t="s">
@@ -633,7 +628,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -658,7 +653,7 @@
       <c r="P2" s="19"/>
       <c r="Q2" s="19"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="9" t="s">
         <v>2</v>
@@ -681,7 +676,7 @@
       <c r="P3" s="19"/>
       <c r="Q3" s="19"/>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="9" t="s">
         <v>3</v>
@@ -706,7 +701,7 @@
       <c r="P4" s="19"/>
       <c r="Q4" s="19"/>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="9" t="s">
         <v>4</v>
@@ -729,7 +724,7 @@
       <c r="P5" s="19"/>
       <c r="Q5" s="19"/>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
@@ -756,7 +751,7 @@
       <c r="P6" s="19"/>
       <c r="Q6" s="19"/>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
       <c r="B7" s="10" t="s">
         <v>2</v>
@@ -781,7 +776,7 @@
       <c r="P7" s="19"/>
       <c r="Q7" s="19"/>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
       <c r="B8" s="10" t="s">
         <v>3</v>
@@ -806,7 +801,7 @@
       <c r="P8" s="19"/>
       <c r="Q8" s="19"/>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
       <c r="B9" s="10" t="s">
         <v>6</v>
@@ -814,7 +809,9 @@
       <c r="C9" s="19">
         <v>0</v>
       </c>
-      <c r="D9" s="19"/>
+      <c r="D9" s="19">
+        <v>0.16666666666666666</v>
+      </c>
       <c r="E9" s="19"/>
       <c r="F9" s="19"/>
       <c r="G9" s="19"/>
@@ -829,7 +826,7 @@
       <c r="P9" s="19"/>
       <c r="Q9" s="19"/>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>8</v>
       </c>
@@ -854,7 +851,7 @@
       <c r="P10" s="19"/>
       <c r="Q10" s="19"/>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C11" s="19"/>
       <c r="D11" s="19"/>
       <c r="E11" s="19"/>
@@ -871,7 +868,7 @@
       <c r="P11" s="19"/>
       <c r="Q11" s="19"/>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
         <v>11</v>
       </c>
@@ -939,7 +936,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="15"/>
       <c r="B13" s="17" t="s">
         <v>2</v>
@@ -1005,7 +1002,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="15"/>
       <c r="B14" s="17" t="s">
         <v>3</v>
@@ -1071,7 +1068,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="16"/>
       <c r="B15" s="17" t="s">
         <v>6</v>
@@ -1082,7 +1079,7 @@
       </c>
       <c r="D15" s="19">
         <f t="shared" ref="D15:E15" si="6">D10+D9+D5</f>
-        <v>0.38541666666666669</v>
+        <v>0.55208333333333337</v>
       </c>
       <c r="E15" s="19">
         <f t="shared" si="6"/>
@@ -1137,10 +1134,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="18"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="19"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added study time of saturday morning-midday
</commit_message>
<xml_diff>
--- a/Uurbesteding.xlsx
+++ b/Uurbesteding.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="465" windowWidth="20415" windowHeight="11940"/>
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -570,7 +570,7 @@
   <dimension ref="A1:Q19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -638,7 +638,9 @@
       <c r="C2" s="19">
         <v>0.25</v>
       </c>
-      <c r="D2" s="19"/>
+      <c r="D2" s="19">
+        <v>0.13541666666666666</v>
+      </c>
       <c r="E2" s="19"/>
       <c r="F2" s="19"/>
       <c r="G2" s="19"/>
@@ -883,7 +885,7 @@
       </c>
       <c r="D12" s="19">
         <f t="shared" ref="D12:E12" si="0">D10+D6+D2</f>
-        <v>0.51041666666666674</v>
+        <v>0.64583333333333337</v>
       </c>
       <c r="E12" s="19">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
Added time for group work saturday
</commit_message>
<xml_diff>
--- a/Uurbesteding.xlsx
+++ b/Uurbesteding.xlsx
@@ -570,7 +570,7 @@
   <dimension ref="A1:Q19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -839,7 +839,7 @@
         <v>0</v>
       </c>
       <c r="D10" s="19">
-        <v>0.38541666666666669</v>
+        <v>0.48958333333333331</v>
       </c>
       <c r="E10" s="19"/>
       <c r="F10" s="19"/>
@@ -885,7 +885,7 @@
       </c>
       <c r="D12" s="19">
         <f t="shared" ref="D12:E12" si="0">D10+D6+D2</f>
-        <v>0.64583333333333337</v>
+        <v>0.74999999999999989</v>
       </c>
       <c r="E12" s="19">
         <f t="shared" si="0"/>
@@ -951,7 +951,7 @@
       </c>
       <c r="D13" s="19">
         <f t="shared" ref="D13:E13" si="2">D10+D7+D3</f>
-        <v>0.61458333333333337</v>
+        <v>0.71875</v>
       </c>
       <c r="E13" s="19">
         <f t="shared" si="2"/>
@@ -1017,7 +1017,7 @@
       </c>
       <c r="D14" s="19">
         <f t="shared" ref="D14:E14" si="4">D10+D8+D4</f>
-        <v>0.55208333333333337</v>
+        <v>0.65624999999999989</v>
       </c>
       <c r="E14" s="19">
         <f t="shared" si="4"/>
@@ -1083,7 +1083,7 @@
       </c>
       <c r="D15" s="19">
         <f t="shared" ref="D15:E15" si="6">D10+D9+D5</f>
-        <v>0.55208333333333337</v>
+        <v>0.65625</v>
       </c>
       <c r="E15" s="19">
         <f t="shared" si="6"/>

</xml_diff>

<commit_message>
ReAdded uurbesteding changes, Mathias overrided my changes
</commit_message>
<xml_diff>
--- a/Uurbesteding.xlsx
+++ b/Uurbesteding.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="26812"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Mathias/Desktop/SwOp-Group03/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="20420" windowHeight="11940"/>
+    <workbookView xWindow="240" yWindow="465" windowWidth="20415" windowHeight="11940"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -270,7 +265,7 @@
     <cellStyle name="Accent3" xfId="2" builtinId="37"/>
     <cellStyle name="Accent4" xfId="3" builtinId="41"/>
     <cellStyle name="Accent6" xfId="4" builtinId="49"/>
-    <cellStyle name="Stand." xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -575,16 +570,16 @@
   <dimension ref="A1:Q19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5" customWidth="1"/>
+    <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="12"/>
       <c r="B1" s="13"/>
       <c r="C1" s="11" t="s">
@@ -633,7 +628,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -660,7 +655,7 @@
       <c r="P2" s="19"/>
       <c r="Q2" s="19"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="9" t="s">
         <v>2</v>
@@ -685,7 +680,7 @@
       <c r="P3" s="19"/>
       <c r="Q3" s="19"/>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="9" t="s">
         <v>3</v>
@@ -710,7 +705,7 @@
       <c r="P4" s="19"/>
       <c r="Q4" s="19"/>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="9" t="s">
         <v>4</v>
@@ -733,7 +728,7 @@
       <c r="P5" s="19"/>
       <c r="Q5" s="19"/>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
@@ -744,7 +739,7 @@
         <v>0</v>
       </c>
       <c r="D6" s="19">
-        <v>0.125</v>
+        <v>0.1875</v>
       </c>
       <c r="E6" s="19"/>
       <c r="F6" s="19"/>
@@ -760,7 +755,7 @@
       <c r="P6" s="19"/>
       <c r="Q6" s="19"/>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
       <c r="B7" s="10" t="s">
         <v>2</v>
@@ -785,7 +780,7 @@
       <c r="P7" s="19"/>
       <c r="Q7" s="19"/>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
       <c r="B8" s="10" t="s">
         <v>3</v>
@@ -810,7 +805,7 @@
       <c r="P8" s="19"/>
       <c r="Q8" s="19"/>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
       <c r="B9" s="10" t="s">
         <v>6</v>
@@ -835,7 +830,7 @@
       <c r="P9" s="19"/>
       <c r="Q9" s="19"/>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>8</v>
       </c>
@@ -860,7 +855,7 @@
       <c r="P10" s="19"/>
       <c r="Q10" s="19"/>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C11" s="19"/>
       <c r="D11" s="19"/>
       <c r="E11" s="19"/>
@@ -877,7 +872,7 @@
       <c r="P11" s="19"/>
       <c r="Q11" s="19"/>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
         <v>11</v>
       </c>
@@ -890,7 +885,7 @@
       </c>
       <c r="D12" s="19">
         <f t="shared" ref="D12:E12" si="0">D10+D6+D2</f>
-        <v>0.74999999999999989</v>
+        <v>0.81249999999999989</v>
       </c>
       <c r="E12" s="19">
         <f t="shared" si="0"/>
@@ -945,7 +940,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="15"/>
       <c r="B13" s="17" t="s">
         <v>2</v>
@@ -1011,7 +1006,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="15"/>
       <c r="B14" s="17" t="s">
         <v>3</v>
@@ -1077,7 +1072,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="16"/>
       <c r="B15" s="17" t="s">
         <v>6</v>
@@ -1143,10 +1138,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="18"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="19"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added hoorcolleges to uurbesteding for completeness
</commit_message>
<xml_diff>
--- a/Uurbesteding.xlsx
+++ b/Uurbesteding.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="25">
   <si>
     <t>studie</t>
   </si>
@@ -91,6 +91,9 @@
   </si>
   <si>
     <t>week 15</t>
+  </si>
+  <si>
+    <t>hoorceollege</t>
   </si>
 </sst>
 </file>
@@ -100,7 +103,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[h]:mm"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -115,14 +118,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF222426"/>
-      <name val="Consolas"/>
-      <family val="3"/>
-    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -149,6 +146,11 @@
         <fgColor theme="9"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="7">
     <border>
@@ -231,14 +233,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="2" applyBorder="1"/>
@@ -257,10 +260,14 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="5" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="5" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="5" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="5" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="6">
+    <cellStyle name="Accent1" xfId="5" builtinId="29"/>
     <cellStyle name="Accent2" xfId="1" builtinId="33"/>
     <cellStyle name="Accent3" xfId="2" builtinId="37"/>
     <cellStyle name="Accent4" xfId="3" builtinId="41"/>
@@ -567,10 +574,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q19"/>
+  <dimension ref="A1:Q20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -635,98 +642,98 @@
       <c r="B2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="19">
+      <c r="C2" s="18">
         <v>0.25</v>
       </c>
-      <c r="D2" s="19">
+      <c r="D2" s="18">
         <v>0.19097222222222221</v>
       </c>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
-      <c r="K2" s="19"/>
-      <c r="L2" s="19"/>
-      <c r="M2" s="19"/>
-      <c r="N2" s="19"/>
-      <c r="O2" s="19"/>
-      <c r="P2" s="19"/>
-      <c r="Q2" s="19"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="18"/>
+      <c r="L2" s="18"/>
+      <c r="M2" s="18"/>
+      <c r="N2" s="18"/>
+      <c r="O2" s="18"/>
+      <c r="P2" s="18"/>
+      <c r="Q2" s="18"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="19">
+      <c r="C3" s="18">
         <v>0.25</v>
       </c>
-      <c r="D3" s="19">
+      <c r="D3" s="18">
         <v>0.24305555555555555</v>
       </c>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
-      <c r="K3" s="19"/>
-      <c r="L3" s="19"/>
-      <c r="M3" s="19"/>
-      <c r="N3" s="19"/>
-      <c r="O3" s="19"/>
-      <c r="P3" s="19"/>
-      <c r="Q3" s="19"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="18"/>
+      <c r="L3" s="18"/>
+      <c r="M3" s="18"/>
+      <c r="N3" s="18"/>
+      <c r="O3" s="18"/>
+      <c r="P3" s="18"/>
+      <c r="Q3" s="18"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="19">
+      <c r="C4" s="18">
         <v>0.125</v>
       </c>
-      <c r="D4" s="19">
+      <c r="D4" s="18">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19"/>
-      <c r="G4" s="19"/>
-      <c r="H4" s="19"/>
-      <c r="I4" s="19"/>
-      <c r="J4" s="19"/>
-      <c r="K4" s="19"/>
-      <c r="L4" s="19"/>
-      <c r="M4" s="19"/>
-      <c r="N4" s="19"/>
-      <c r="O4" s="19"/>
-      <c r="P4" s="19"/>
-      <c r="Q4" s="19"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="18"/>
+      <c r="I4" s="18"/>
+      <c r="J4" s="18"/>
+      <c r="K4" s="18"/>
+      <c r="L4" s="18"/>
+      <c r="M4" s="18"/>
+      <c r="N4" s="18"/>
+      <c r="O4" s="18"/>
+      <c r="P4" s="18"/>
+      <c r="Q4" s="18"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="19">
+      <c r="C5" s="18">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="19"/>
-      <c r="H5" s="19"/>
-      <c r="I5" s="19"/>
-      <c r="J5" s="19"/>
-      <c r="K5" s="19"/>
-      <c r="L5" s="19"/>
-      <c r="M5" s="19"/>
-      <c r="N5" s="19"/>
-      <c r="O5" s="19"/>
-      <c r="P5" s="19"/>
-      <c r="Q5" s="19"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="18"/>
+      <c r="I5" s="18"/>
+      <c r="J5" s="18"/>
+      <c r="K5" s="18"/>
+      <c r="L5" s="18"/>
+      <c r="M5" s="18"/>
+      <c r="N5" s="18"/>
+      <c r="O5" s="18"/>
+      <c r="P5" s="18"/>
+      <c r="Q5" s="18"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
@@ -735,414 +742,470 @@
       <c r="B6" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="19">
-        <v>0</v>
-      </c>
-      <c r="D6" s="19">
+      <c r="C6" s="18">
+        <v>0</v>
+      </c>
+      <c r="D6" s="18">
         <v>0.1875</v>
       </c>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="19"/>
-      <c r="H6" s="19"/>
-      <c r="I6" s="19"/>
-      <c r="J6" s="19"/>
-      <c r="K6" s="19"/>
-      <c r="L6" s="19"/>
-      <c r="M6" s="19"/>
-      <c r="N6" s="19"/>
-      <c r="O6" s="19"/>
-      <c r="P6" s="19"/>
-      <c r="Q6" s="19"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="18"/>
+      <c r="K6" s="18"/>
+      <c r="L6" s="18"/>
+      <c r="M6" s="18"/>
+      <c r="N6" s="18"/>
+      <c r="O6" s="18"/>
+      <c r="P6" s="18"/>
+      <c r="Q6" s="18"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
       <c r="B7" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="19">
-        <v>0</v>
-      </c>
-      <c r="D7" s="19">
+      <c r="C7" s="18">
+        <v>0</v>
+      </c>
+      <c r="D7" s="18">
         <v>0.16666666666666666</v>
       </c>
-      <c r="E7" s="19"/>
-      <c r="F7" s="19"/>
-      <c r="G7" s="19"/>
-      <c r="H7" s="19"/>
-      <c r="I7" s="19"/>
-      <c r="J7" s="19"/>
-      <c r="K7" s="19"/>
-      <c r="L7" s="19"/>
-      <c r="M7" s="19"/>
-      <c r="N7" s="19"/>
-      <c r="O7" s="19"/>
-      <c r="P7" s="19"/>
-      <c r="Q7" s="19"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="18"/>
+      <c r="J7" s="18"/>
+      <c r="K7" s="18"/>
+      <c r="L7" s="18"/>
+      <c r="M7" s="18"/>
+      <c r="N7" s="18"/>
+      <c r="O7" s="18"/>
+      <c r="P7" s="18"/>
+      <c r="Q7" s="18"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
       <c r="B8" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="19">
-        <v>0</v>
-      </c>
-      <c r="D8" s="19">
+      <c r="C8" s="18">
+        <v>0</v>
+      </c>
+      <c r="D8" s="18">
         <v>0.16666666666666666</v>
       </c>
-      <c r="E8" s="19"/>
-      <c r="F8" s="19"/>
-      <c r="G8" s="19"/>
-      <c r="H8" s="19"/>
-      <c r="I8" s="19"/>
-      <c r="J8" s="19"/>
-      <c r="K8" s="19"/>
-      <c r="L8" s="19"/>
-      <c r="M8" s="19"/>
-      <c r="N8" s="19"/>
-      <c r="O8" s="19"/>
-      <c r="P8" s="19"/>
-      <c r="Q8" s="19"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="18"/>
+      <c r="I8" s="18"/>
+      <c r="J8" s="18"/>
+      <c r="K8" s="18"/>
+      <c r="L8" s="18"/>
+      <c r="M8" s="18"/>
+      <c r="N8" s="18"/>
+      <c r="O8" s="18"/>
+      <c r="P8" s="18"/>
+      <c r="Q8" s="18"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
       <c r="B9" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="19">
-        <v>0</v>
-      </c>
-      <c r="D9" s="19">
+      <c r="C9" s="18">
+        <v>0</v>
+      </c>
+      <c r="D9" s="18">
         <v>0.16666666666666666</v>
       </c>
-      <c r="E9" s="19"/>
-      <c r="F9" s="19"/>
-      <c r="G9" s="19"/>
-      <c r="H9" s="19"/>
-      <c r="I9" s="19"/>
-      <c r="J9" s="19"/>
-      <c r="K9" s="19"/>
-      <c r="L9" s="19"/>
-      <c r="M9" s="19"/>
-      <c r="N9" s="19"/>
-      <c r="O9" s="19"/>
-      <c r="P9" s="19"/>
-      <c r="Q9" s="19"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="18"/>
+      <c r="J9" s="18"/>
+      <c r="K9" s="18"/>
+      <c r="L9" s="18"/>
+      <c r="M9" s="18"/>
+      <c r="N9" s="18"/>
+      <c r="O9" s="18"/>
+      <c r="P9" s="18"/>
+      <c r="Q9" s="18"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="8"/>
-      <c r="C10" s="19">
-        <v>0</v>
-      </c>
-      <c r="D10" s="19">
+      <c r="C10" s="18">
+        <v>0</v>
+      </c>
+      <c r="D10" s="18">
         <v>0.48958333333333331</v>
       </c>
-      <c r="E10" s="19"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="19"/>
-      <c r="H10" s="19"/>
-      <c r="I10" s="19"/>
-      <c r="J10" s="19"/>
-      <c r="K10" s="19"/>
-      <c r="L10" s="19"/>
-      <c r="M10" s="19"/>
-      <c r="N10" s="19"/>
-      <c r="O10" s="19"/>
-      <c r="P10" s="19"/>
-      <c r="Q10" s="19"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="18"/>
+      <c r="J10" s="18"/>
+      <c r="K10" s="18"/>
+      <c r="L10" s="18"/>
+      <c r="M10" s="18"/>
+      <c r="N10" s="18"/>
+      <c r="O10" s="18"/>
+      <c r="P10" s="18"/>
+      <c r="Q10" s="18"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="C11" s="19"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="19"/>
-      <c r="F11" s="19"/>
-      <c r="G11" s="19"/>
-      <c r="H11" s="19"/>
-      <c r="I11" s="19"/>
-      <c r="J11" s="19"/>
-      <c r="K11" s="19"/>
-      <c r="L11" s="19"/>
-      <c r="M11" s="19"/>
-      <c r="N11" s="19"/>
-      <c r="O11" s="19"/>
-      <c r="P11" s="19"/>
-      <c r="Q11" s="19"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="18"/>
+      <c r="I11" s="18"/>
+      <c r="J11" s="18"/>
+      <c r="K11" s="18"/>
+      <c r="L11" s="18"/>
+      <c r="M11" s="18"/>
+      <c r="N11" s="18"/>
+      <c r="O11" s="18"/>
+      <c r="P11" s="18"/>
+      <c r="Q11" s="18"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" s="14" t="s">
+      <c r="A12" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="18">
+        <v>0</v>
+      </c>
+      <c r="D12" s="18">
+        <v>6.25E-2</v>
+      </c>
+      <c r="E12" s="18">
+        <v>6.25E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A13" s="21"/>
+      <c r="B13" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" s="18">
+        <v>0</v>
+      </c>
+      <c r="D13" s="18">
+        <v>6.25E-2</v>
+      </c>
+      <c r="E13" s="18">
+        <v>6.25E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A14" s="21"/>
+      <c r="B14" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="18">
+        <v>0</v>
+      </c>
+      <c r="D14" s="18">
+        <v>6.25E-2</v>
+      </c>
+      <c r="E14" s="18">
+        <v>6.25E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A15" s="22"/>
+      <c r="B15" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="18">
+        <v>0</v>
+      </c>
+      <c r="D15" s="18">
+        <v>6.25E-2</v>
+      </c>
+      <c r="E15" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A17" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="17" t="s">
+      <c r="B17" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="19">
-        <f>C10+C6+C2</f>
+      <c r="C17" s="18">
+        <f>C10+C6+C2+C12</f>
         <v>0.25</v>
       </c>
-      <c r="D12" s="19">
-        <f t="shared" ref="D12:E12" si="0">D10+D6+D2</f>
-        <v>0.86805555555555547</v>
-      </c>
-      <c r="E12" s="19">
+      <c r="D17" s="18">
+        <f>D10+D6+D2+D12</f>
+        <v>0.93055555555555547</v>
+      </c>
+      <c r="E17" s="18">
+        <f>E10+E6+E2+E12</f>
+        <v>6.25E-2</v>
+      </c>
+      <c r="F17" s="18">
+        <f t="shared" ref="F17:Q17" si="0">F10+F6+F2+F12</f>
+        <v>0</v>
+      </c>
+      <c r="G17" s="18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F12" s="19">
-        <f t="shared" ref="F12:Q12" si="1">F10+F6+F2</f>
-        <v>0</v>
-      </c>
-      <c r="G12" s="19">
+      <c r="H17" s="18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I17" s="18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J17" s="18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K17" s="18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L17" s="18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M17" s="18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N17" s="18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O17" s="18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P17" s="18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q17" s="18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A18" s="15"/>
+      <c r="B18" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="C18" s="18">
+        <f>C10+C7+C3+C13</f>
+        <v>0.25</v>
+      </c>
+      <c r="D18" s="18">
+        <f>D10+D7+D3+D13</f>
+        <v>0.96180555555555558</v>
+      </c>
+      <c r="E18" s="18">
+        <f>E10+E7+E3+E13</f>
+        <v>6.25E-2</v>
+      </c>
+      <c r="F18" s="18">
+        <f t="shared" ref="F18:Q18" si="1">F10+F7+F3+F13</f>
+        <v>0</v>
+      </c>
+      <c r="G18" s="18">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H12" s="19">
+      <c r="H18" s="18">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I12" s="19">
+      <c r="I18" s="18">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J12" s="19">
+      <c r="J18" s="18">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K12" s="19">
+      <c r="K18" s="18">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L12" s="19">
+      <c r="L18" s="18">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M12" s="19">
+      <c r="M18" s="18">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="N12" s="19">
+      <c r="N18" s="18">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O12" s="19">
+      <c r="O18" s="18">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="P12" s="19">
+      <c r="P18" s="18">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Q12" s="19">
+      <c r="Q18" s="18">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" s="15"/>
-      <c r="B13" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="C13" s="19">
-        <f>C10+C7+C3</f>
-        <v>0.25</v>
-      </c>
-      <c r="D13" s="19">
-        <f t="shared" ref="D13:E13" si="2">D10+D7+D3</f>
-        <v>0.89930555555555558</v>
-      </c>
-      <c r="E13" s="19">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A19" s="15"/>
+      <c r="B19" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" s="18">
+        <f>C10+C8+C4+C14</f>
+        <v>0.125</v>
+      </c>
+      <c r="D19" s="18">
+        <f>D10+D8+D4+D14</f>
+        <v>0.80208333333333337</v>
+      </c>
+      <c r="E19" s="18">
+        <f>E10+E8+E4+E14</f>
+        <v>6.25E-2</v>
+      </c>
+      <c r="F19" s="18">
+        <f t="shared" ref="F19:Q19" si="2">F10+F8+F4+F14</f>
+        <v>0</v>
+      </c>
+      <c r="G19" s="18">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F13" s="19">
-        <f t="shared" ref="F13:Q13" si="3">F10+F7+F3</f>
-        <v>0</v>
-      </c>
-      <c r="G13" s="19">
+      <c r="H19" s="18">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I19" s="18">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J19" s="18">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K19" s="18">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L19" s="18">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M19" s="18">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N19" s="18">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O19" s="18">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P19" s="18">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q19" s="18">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A20" s="16"/>
+      <c r="B20" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" s="18">
+        <f>C10+C9+C5+C15</f>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D20" s="18">
+        <f>D10+D9+D5+D15</f>
+        <v>0.71875</v>
+      </c>
+      <c r="E20" s="18">
+        <f>E10+E9+E5+E15</f>
+        <v>0</v>
+      </c>
+      <c r="F20" s="18">
+        <f t="shared" ref="F20:Q20" si="3">F10+F9+F5+F15</f>
+        <v>0</v>
+      </c>
+      <c r="G20" s="18">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="H13" s="19">
+      <c r="H20" s="18">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="I13" s="19">
+      <c r="I20" s="18">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J13" s="19">
+      <c r="J20" s="18">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="K13" s="19">
+      <c r="K20" s="18">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="L13" s="19">
+      <c r="L20" s="18">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M13" s="19">
+      <c r="M20" s="18">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="N13" s="19">
+      <c r="N20" s="18">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="O13" s="19">
+      <c r="O20" s="18">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="P13" s="19">
+      <c r="P20" s="18">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="Q13" s="19">
+      <c r="Q20" s="18">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A14" s="15"/>
-      <c r="B14" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="C14" s="19">
-        <f>C10+C8+C4</f>
-        <v>0.125</v>
-      </c>
-      <c r="D14" s="19">
-        <f t="shared" ref="D14:E14" si="4">D10+D8+D4</f>
-        <v>0.73958333333333337</v>
-      </c>
-      <c r="E14" s="19">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="F14" s="19">
-        <f t="shared" ref="F14:Q14" si="5">F10+F8+F4</f>
-        <v>0</v>
-      </c>
-      <c r="G14" s="19">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="H14" s="19">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="I14" s="19">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="J14" s="19">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="K14" s="19">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="L14" s="19">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="M14" s="19">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="N14" s="19">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="O14" s="19">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="P14" s="19">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="Q14" s="19">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" s="16"/>
-      <c r="B15" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15" s="19">
-        <f>C10+C9+C5</f>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="D15" s="19">
-        <f t="shared" ref="D15:E15" si="6">D10+D9+D5</f>
-        <v>0.65625</v>
-      </c>
-      <c r="E15" s="19">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="F15" s="19">
-        <f t="shared" ref="F15:Q15" si="7">F10+F9+F5</f>
-        <v>0</v>
-      </c>
-      <c r="G15" s="19">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="H15" s="19">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="I15" s="19">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="J15" s="19">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="K15" s="19">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="L15" s="19">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="M15" s="19">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="N15" s="19">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="O15" s="19">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="P15" s="19">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="Q15" s="19">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="18"/>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added time for group work on 22-02-2016
</commit_message>
<xml_diff>
--- a/Uurbesteding.xlsx
+++ b/Uurbesteding.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="26812"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Mathias/Desktop/SwOp-Group03/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="20420" windowHeight="11940"/>
+    <workbookView xWindow="240" yWindow="465" windowWidth="20415" windowHeight="11940"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -277,7 +272,7 @@
     <cellStyle name="Accent3" xfId="2" builtinId="37"/>
     <cellStyle name="Accent4" xfId="3" builtinId="41"/>
     <cellStyle name="Accent6" xfId="4" builtinId="49"/>
-    <cellStyle name="Stand." xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -582,16 +577,16 @@
   <dimension ref="A1:Q20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5" customWidth="1"/>
+    <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="12"/>
       <c r="B1" s="13"/>
       <c r="C1" s="11" t="s">
@@ -640,7 +635,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -667,7 +662,7 @@
       <c r="P2" s="18"/>
       <c r="Q2" s="18"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="9" t="s">
         <v>2</v>
@@ -692,7 +687,7 @@
       <c r="P3" s="18"/>
       <c r="Q3" s="18"/>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="9" t="s">
         <v>3</v>
@@ -717,7 +712,7 @@
       <c r="P4" s="18"/>
       <c r="Q4" s="18"/>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="9" t="s">
         <v>4</v>
@@ -740,7 +735,7 @@
       <c r="P5" s="18"/>
       <c r="Q5" s="18"/>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
@@ -767,7 +762,7 @@
       <c r="P6" s="18"/>
       <c r="Q6" s="18"/>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
       <c r="B7" s="10" t="s">
         <v>2</v>
@@ -792,7 +787,7 @@
       <c r="P7" s="18"/>
       <c r="Q7" s="18"/>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
       <c r="B8" s="10" t="s">
         <v>3</v>
@@ -817,7 +812,7 @@
       <c r="P8" s="18"/>
       <c r="Q8" s="18"/>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
       <c r="B9" s="10" t="s">
         <v>6</v>
@@ -842,7 +837,7 @@
       <c r="P9" s="18"/>
       <c r="Q9" s="18"/>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>8</v>
       </c>
@@ -853,7 +848,9 @@
       <c r="D10" s="18">
         <v>0.48958333333333331</v>
       </c>
-      <c r="E10" s="18"/>
+      <c r="E10" s="18">
+        <v>0.16666666666666666</v>
+      </c>
       <c r="F10" s="18"/>
       <c r="G10" s="18"/>
       <c r="H10" s="18"/>
@@ -867,7 +864,7 @@
       <c r="P10" s="18"/>
       <c r="Q10" s="18"/>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C11" s="18"/>
       <c r="D11" s="18"/>
       <c r="E11" s="18"/>
@@ -884,7 +881,7 @@
       <c r="P11" s="18"/>
       <c r="Q11" s="18"/>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="19" t="s">
         <v>24</v>
       </c>
@@ -901,7 +898,7 @@
         <v>6.25E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="21"/>
       <c r="B13" s="20" t="s">
         <v>2</v>
@@ -916,7 +913,7 @@
         <v>6.25E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="21"/>
       <c r="B14" s="20" t="s">
         <v>3</v>
@@ -931,7 +928,7 @@
         <v>6.25E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="22"/>
       <c r="B15" s="20" t="s">
         <v>6</v>
@@ -946,7 +943,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
         <v>11</v>
       </c>
@@ -963,7 +960,7 @@
       </c>
       <c r="E17" s="18">
         <f>E10+E6+E2+E12</f>
-        <v>6.25E-2</v>
+        <v>0.22916666666666666</v>
       </c>
       <c r="F17" s="18">
         <f t="shared" ref="F17:Q17" si="0">F10+F6+F2+F12</f>
@@ -1014,7 +1011,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="15"/>
       <c r="B18" s="17" t="s">
         <v>2</v>
@@ -1029,7 +1026,7 @@
       </c>
       <c r="E18" s="18">
         <f>E10+E7+E3+E13</f>
-        <v>6.25E-2</v>
+        <v>0.22916666666666666</v>
       </c>
       <c r="F18" s="18">
         <f t="shared" ref="F18:Q18" si="1">F10+F7+F3+F13</f>
@@ -1080,7 +1077,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="15"/>
       <c r="B19" s="17" t="s">
         <v>3</v>
@@ -1095,7 +1092,7 @@
       </c>
       <c r="E19" s="18">
         <f>E10+E8+E4+E14</f>
-        <v>6.25E-2</v>
+        <v>0.22916666666666666</v>
       </c>
       <c r="F19" s="18">
         <f t="shared" ref="F19:Q19" si="2">F10+F8+F4+F14</f>
@@ -1146,7 +1143,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="16"/>
       <c r="B20" s="17" t="s">
         <v>6</v>
@@ -1161,7 +1158,7 @@
       </c>
       <c r="E20" s="18">
         <f>E10+E9+E5+E15</f>
-        <v>0</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="F20" s="18">
         <f t="shared" ref="F20:Q20" si="3">F10+F9+F5+F15</f>

</xml_diff>

<commit_message>
Made changes to uurbesteding.xlsx
</commit_message>
<xml_diff>
--- a/Uurbesteding.xlsx
+++ b/Uurbesteding.xlsx
@@ -577,7 +577,7 @@
   <dimension ref="A1:Q20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -749,7 +749,7 @@
         <v>0.1875</v>
       </c>
       <c r="E6" s="18">
-        <v>7.2916666666666671E-2</v>
+        <v>9.375E-2</v>
       </c>
       <c r="F6" s="18"/>
       <c r="G6" s="18"/>
@@ -962,7 +962,7 @@
       </c>
       <c r="E17" s="18">
         <f>E10+E6+E2+E12</f>
-        <v>0.30208333333333331</v>
+        <v>0.32291666666666663</v>
       </c>
       <c r="F17" s="18">
         <f t="shared" ref="F17:Q17" si="0">F10+F6+F2+F12</f>

</xml_diff>

<commit_message>
Added time to uurbesteding for Ben and Vincent
</commit_message>
<xml_diff>
--- a/Uurbesteding.xlsx
+++ b/Uurbesteding.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="465" windowWidth="20415" windowHeight="11940"/>
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -577,7 +577,7 @@
   <dimension ref="A1:Q20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -749,7 +749,7 @@
         <v>0.1875</v>
       </c>
       <c r="E6" s="18">
-        <v>9.375E-2</v>
+        <v>0.30208333333333331</v>
       </c>
       <c r="F6" s="18"/>
       <c r="G6" s="18"/>
@@ -776,7 +776,7 @@
         <v>0.16666666666666666</v>
       </c>
       <c r="E7" s="18">
-        <v>6.25E-2</v>
+        <v>0.27083333333333331</v>
       </c>
       <c r="F7" s="18"/>
       <c r="G7" s="18"/>
@@ -964,7 +964,7 @@
       </c>
       <c r="E17" s="18">
         <f>E10+E6+E2+E12</f>
-        <v>0.48958333333333331</v>
+        <v>0.69791666666666663</v>
       </c>
       <c r="F17" s="18">
         <f t="shared" ref="F17:Q17" si="0">F10+F6+F2+F12</f>
@@ -1030,7 +1030,7 @@
       </c>
       <c r="E18" s="18">
         <f>E10+E7+E3+E13</f>
-        <v>0.45833333333333331</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="F18" s="18">
         <f t="shared" ref="F18:Q18" si="1">F10+F7+F3+F13</f>

</xml_diff>

<commit_message>
Added oefz tijd to uurbesteding
</commit_message>
<xml_diff>
--- a/Uurbesteding.xlsx
+++ b/Uurbesteding.xlsx
@@ -577,7 +577,7 @@
   <dimension ref="A1:Q20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -896,10 +896,10 @@
         <v>0</v>
       </c>
       <c r="D12" s="18">
-        <v>6.25E-2</v>
+        <v>0.10416666666666667</v>
       </c>
       <c r="E12" s="18">
-        <v>6.25E-2</v>
+        <v>0.16666666666666666</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
@@ -911,10 +911,10 @@
         <v>0</v>
       </c>
       <c r="D13" s="18">
-        <v>6.25E-2</v>
+        <v>0.10416666666666667</v>
       </c>
       <c r="E13" s="18">
-        <v>6.25E-2</v>
+        <v>0.16666666666666666</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
@@ -926,10 +926,10 @@
         <v>0</v>
       </c>
       <c r="D14" s="18">
-        <v>6.25E-2</v>
+        <v>0.10416666666666667</v>
       </c>
       <c r="E14" s="18">
-        <v>6.25E-2</v>
+        <v>0.16666666666666666</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
@@ -941,10 +941,10 @@
         <v>0</v>
       </c>
       <c r="D15" s="18">
-        <v>6.25E-2</v>
+        <v>0.10416666666666667</v>
       </c>
       <c r="E15" s="18">
-        <v>0</v>
+        <v>0.10416666666666667</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
@@ -960,11 +960,11 @@
       </c>
       <c r="D17" s="18">
         <f>D10+D6+D2+D12</f>
-        <v>0.93055555555555547</v>
+        <v>0.9722222222222221</v>
       </c>
       <c r="E17" s="18">
         <f>E10+E6+E2+E12</f>
-        <v>0.69791666666666663</v>
+        <v>0.80208333333333326</v>
       </c>
       <c r="F17" s="18">
         <f t="shared" ref="F17:Q17" si="0">F10+F6+F2+F12</f>
@@ -1026,11 +1026,11 @@
       </c>
       <c r="D18" s="18">
         <f>D10+D7+D3+D13</f>
-        <v>0.96180555555555558</v>
+        <v>1.0034722222222223</v>
       </c>
       <c r="E18" s="18">
         <f>E10+E7+E3+E13</f>
-        <v>0.66666666666666663</v>
+        <v>0.77083333333333326</v>
       </c>
       <c r="F18" s="18">
         <f t="shared" ref="F18:Q18" si="1">F10+F7+F3+F13</f>
@@ -1092,11 +1092,11 @@
       </c>
       <c r="D19" s="18">
         <f>D10+D8+D4+D14</f>
-        <v>0.84375</v>
+        <v>0.88541666666666663</v>
       </c>
       <c r="E19" s="18">
         <f>E10+E8+E4+E14</f>
-        <v>0.39583333333333331</v>
+        <v>0.5</v>
       </c>
       <c r="F19" s="18">
         <f t="shared" ref="F19:Q19" si="2">F10+F8+F4+F14</f>
@@ -1158,11 +1158,11 @@
       </c>
       <c r="D20" s="18">
         <f>D10+D9+D5+D15</f>
-        <v>0.71875</v>
+        <v>0.76041666666666663</v>
       </c>
       <c r="E20" s="18">
         <f>E10+E9+E5+E15</f>
-        <v>0.33333333333333331</v>
+        <v>0.4375</v>
       </c>
       <c r="F20" s="18">
         <f t="shared" ref="F20:Q20" si="3">F10+F9+F5+F15</f>

</xml_diff>